<commit_message>
add commit, update readme, tune parameters, add figures
</commit_message>
<xml_diff>
--- a/systemparameter/para.xlsx
+++ b/systemparameter/para.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6c93646d459ac18/桌面/MATLAB/Projects/Motor.BearingDynamicsModelling/systemparameter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6c93646d459ac18/桌面/master/故障诊断/Bearing-Dynamics/systemparameter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="11_F25DC773A252ABDACC10480C091B54725ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A08AD98-1315-440E-8D6A-208D8E220715}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC10480C091B54725ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A5DBA71-CF0A-41BD-B696-CC26D531A4F0}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="23064" windowHeight="12472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="2085" windowWidth="21600" windowHeight="11393" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Bearing</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,14 +139,6 @@
   </si>
   <si>
     <t>Length(degree)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Motor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unbalance Magnetic Pull</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -174,17 +166,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -245,15 +237,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -266,6 +258,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,38 +530,38 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.7" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.46484375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.1328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.53125" style="1" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="35.21875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="24.1328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="35.19921875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -592,21 +588,21 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="4">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4">
-        <v>100000</v>
+        <v>2000000</v>
       </c>
       <c r="D3" s="4">
-        <v>100000</v>
+        <v>2000000</v>
       </c>
       <c r="E3" s="4">
-        <v>0.63</v>
+        <v>2E-3</v>
       </c>
       <c r="F3" s="4">
         <f>0.05/2</f>
@@ -621,7 +617,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -632,20 +628,20 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -672,7 +668,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" s="4">
         <v>0.5</v>
       </c>
@@ -686,10 +682,10 @@
         <v>100000000</v>
       </c>
       <c r="E7" s="4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F7" s="4">
-        <v>79.75</v>
+        <v>81.494100000000003</v>
       </c>
       <c r="G7" s="4">
         <v>9.8000000000000007</v>
@@ -699,7 +695,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -710,7 +706,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -721,20 +717,20 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:10">
+      <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -749,12 +745,12 @@
       <c r="H11" s="4"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12" s="4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B12" s="4">
-        <v>5.0000000000000002E-5</v>
+        <v>1.9999999999999999E-6</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -764,7 +760,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -775,23 +771,23 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:10">
+      <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
@@ -810,14 +806,14 @@
       <c r="H15" s="4"/>
       <c r="I15" s="2"/>
       <c r="J15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="4">
         <v>1</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C16" s="4">
@@ -832,10 +828,10 @@
       <c r="H16" s="4"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -846,10 +842,8 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>26</v>
-      </c>
+    <row r="18" spans="1:10">
+      <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -859,13 +853,11 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="4"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -875,13 +867,11 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="4"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -891,7 +881,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="14.3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>

</xml_diff>